<commit_message>
Added Elevation values and Jamming periods
</commit_message>
<xml_diff>
--- a/Data/Jamming.xlsx
+++ b/Data/Jamming.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
     <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
     <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="73">
   <si>
     <t>Power (dbm)</t>
   </si>
@@ -236,6 +237,12 @@
   </si>
   <si>
     <t>CW</t>
+  </si>
+  <si>
+    <t>End time</t>
+  </si>
+  <si>
+    <t>Start Time</t>
   </si>
 </sst>
 </file>
@@ -280,10 +287,10 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +764,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.42083333333333334</v>
       </c>
       <c r="E2" t="s">
@@ -842,6 +849,86 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.58472222222222225</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.58576388888888886</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.58750000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.58969907407407407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -850,7 +937,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +1054,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,14 +1271,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1596,7 +1683,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>